<commit_message>
renaming of risk driver 2
</commit_message>
<xml_diff>
--- a/Data/Expert_weights.xlsx
+++ b/Data/Expert_weights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IrisReitsmaRiskQuest\Documents\GitHub\dasbhoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257500C3-05F9-4CF9-8EF2-C0E557F9D76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE7862F-674F-4BCB-9CFC-1DFFFF1B72BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B959621-CE8C-40AE-BCFC-16B25DBD14E7}"/>
+    <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{7B959621-CE8C-40AE-BCFC-16B25DBD14E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Ability of Management Team</t>
   </si>
   <si>
-    <t>Suitability of product for Circularity</t>
-  </si>
-  <si>
     <t>Circularity of asset</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>Security of resources</t>
+  </si>
+  <si>
+    <t>Suitability for circular proposition</t>
   </si>
 </sst>
 </file>
@@ -431,34 +431,34 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="46.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -480,7 +480,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>11</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>3.6666666666666665</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>13.666666666666666</v>

</xml_diff>

<commit_message>
changes in wording of riskdrivers and text
</commit_message>
<xml_diff>
--- a/Data/Expert_weights.xlsx
+++ b/Data/Expert_weights.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE7862F-674F-4BCB-9CFC-1DFFFF1B72BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501D6CBE-9144-47A3-ACB6-FC1D35FABF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{7B959621-CE8C-40AE-BCFC-16B25DBD14E7}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>